<commit_message>
fix: Imported module student, majors, subjects and subjects to major
</commit_message>
<xml_diff>
--- a/public/assets/excels/template-majors.xlsx
+++ b/public/assets/excels/template-majors.xlsx
@@ -1,33 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smart\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qlokappsdev/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41A701F-CE7D-4B59-A4F1-86118B8B2260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7127AEED-F730-FD4A-9175-4CCEAB98FFA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{F3FA2B34-D970-403C-8F21-F3EB3AEE8AD0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{F3FA2B34-D970-403C-8F21-F3EB3AEE8AD0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Lembar1" sheetId="1" r:id="rId1"/>
+    <sheet name="Majors" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -36,15 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="38">
   <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Level</t>
-  </si>
-  <si>
     <t>Agribisnis Bidang Minat Penyuluhan dan Komunikasi</t>
   </si>
   <si>
@@ -148,6 +130,15 @@
   </si>
   <si>
     <t>Perpajakan</t>
+  </si>
+  <si>
+    <t>Kode Jurusan</t>
+  </si>
+  <si>
+    <t>Jurusan</t>
+  </si>
+  <si>
+    <t>Jenjang</t>
   </si>
 </sst>
 </file>
@@ -227,7 +218,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -525,377 +516,378 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30C1E682-9314-47F4-BE19-DD3710FF72ED}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
     <col min="2" max="2" width="68.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>77</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>74</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>75</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>83</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>78</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>53</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>458</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>51</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>50</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>311</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>72</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>71</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>310</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>38</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>54</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>55</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>57</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>58</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>59</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>76</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>60</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>61</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>62</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>73</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>279</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>30</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>87</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>252</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>70</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>56</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>84</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>163</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>